<commit_message>
Db Extraction  and Db validation integrated
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestData/DataSheet/TestData.xlsx
+++ b/src/main/resources/InputTestData/DataSheet/TestData.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="84">
   <si>
     <t>RunFlag</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>p_id</t>
   </si>
   <si>
     <t>y</t>
@@ -141,7 +144,13 @@
 }</t>
   </si>
   <si>
-    <t>no</t>
+    <t>GetProduct</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>created_at</t>
   </si>
   <si>
     <t>eve.holt@reqres.in</t>
@@ -190,6 +199,9 @@
 }</t>
   </si>
   <si>
+    <t>no</t>
+  </si>
+  <si>
     <t>hello</t>
   </si>
   <si>
@@ -214,124 +226,67 @@
     <t/>
   </si>
   <si>
-    <t>688</t>
-  </si>
-  <si>
-    <t>730</t>
-  </si>
-  <si>
-    <t>267</t>
-  </si>
-  <si>
-    <t>139</t>
-  </si>
-  <si>
-    <t>986</t>
-  </si>
-  <si>
-    <t>136</t>
-  </si>
-  <si>
-    <t>452</t>
-  </si>
-  <si>
-    <t>915</t>
-  </si>
-  <si>
-    <t>212</t>
-  </si>
-  <si>
-    <t>616</t>
-  </si>
-  <si>
-    <t>545</t>
-  </si>
-  <si>
-    <t>697</t>
-  </si>
-  <si>
-    <t>575</t>
-  </si>
-  <si>
-    <t>708</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>469</t>
-  </si>
-  <si>
-    <t>182</t>
-  </si>
-  <si>
-    <t>439</t>
-  </si>
-  <si>
-    <t>711</t>
-  </si>
-  <si>
-    <t>174</t>
-  </si>
-  <si>
-    <t>164</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>96</t>
-  </si>
-  <si>
-    <t>686</t>
-  </si>
-  <si>
-    <t>540</t>
-  </si>
-  <si>
-    <t>916</t>
-  </si>
-  <si>
-    <t>67</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>561</t>
-  </si>
-  <si>
-    <t>732</t>
-  </si>
-  <si>
-    <t>492</t>
-  </si>
-  <si>
-    <t>341</t>
-  </si>
-  <si>
-    <t>445</t>
-  </si>
-  <si>
-    <t>842</t>
-  </si>
-  <si>
-    <t>761</t>
-  </si>
-  <si>
-    <t>235</t>
-  </si>
-  <si>
-    <t>365</t>
+    <t>4</t>
+  </si>
+  <si>
+    <t>696</t>
   </si>
   <si>
     <t>921</t>
   </si>
   <si>
-    <t>256</t>
-  </si>
-  <si>
-    <t>497</t>
+    <t>350</t>
+  </si>
+  <si>
+    <t>883</t>
+  </si>
+  <si>
+    <t>309</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>778</t>
+  </si>
+  <si>
+    <t>504</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>265</t>
+  </si>
+  <si>
+    <t>408</t>
+  </si>
+  <si>
+    <t>614</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>313</t>
+  </si>
+  <si>
+    <t>431</t>
+  </si>
+  <si>
+    <t>443</t>
+  </si>
+  <si>
+    <t>769</t>
+  </si>
+  <si>
+    <t>963</t>
+  </si>
+  <si>
+    <t>563</t>
+  </si>
+  <si>
+    <t>122</t>
   </si>
 </sst>
 </file>
@@ -382,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -403,6 +358,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -720,7 +678,9 @@
       <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="4"/>
+      <c r="AC1" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="AD1" s="4"/>
       <c r="AE1" s="4"/>
       <c r="AF1" s="4"/>
@@ -729,34 +689,34 @@
     </row>
     <row r="2" ht="45.0" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>24</v>
@@ -765,149 +725,165 @@
         <v>200.0</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="X2" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Z2" t="s" s="0">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AA2" t="s" s="0">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AB2" t="s" s="0">
-        <v>58</v>
+        <v>62</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="3" ht="45.0" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="N3" s="5">
         <v>201.0</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="W3" t="s" s="0">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="X3" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="Y3" s="7" t="str">
+        <v>62</v>
+      </c>
+      <c r="Y3" s="8" t="str">
         <f t="shared" ref="Y3:Y4" si="1">Y2</f>
         <v>a</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>98</v>
+        <v>83</v>
+      </c>
+      <c r="AC3" t="s" s="0">
+        <v>62</v>
       </c>
     </row>
     <row r="4" ht="45.0" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="N4" s="5">
         <v>204.0</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="W4" t="s" s="0">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="X4" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="Y4" s="7" t="str">
+        <v>62</v>
+      </c>
+      <c r="Y4" s="8" t="str">
         <f t="shared" si="1"/>
         <v>a</v>
       </c>
       <c r="Z4" t="s" s="0">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AA4" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="AB4" s="7" t="str">
+        <v>62</v>
+      </c>
+      <c r="AB4" s="8" t="str">
         <f>AB3</f>
         <v>as</v>
       </c>
+      <c r="AC4" t="s" s="0">
+        <v>62</v>
+      </c>
     </row>
     <row r="5">
-      <c r="E5" s="5" t="s">
-        <v>56</v>
-      </c>
+      <c r="E5" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Request Extract feature added
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestData/DataSheet/TestData.xlsx
+++ b/src/main/resources/InputTestData/DataSheet/TestData.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="85">
   <si>
     <t>RunFlag</t>
   </si>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t>122</t>
+  </si>
+  <si>
+    <t>779</t>
   </si>
 </sst>
 </file>
@@ -821,7 +824,7 @@
         <v>56</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AC3" t="s" s="0">
         <v>62</v>

</xml_diff>

<commit_message>
added test info for extent report
</commit_message>
<xml_diff>
--- a/src/main/resources/InputTestData/DataSheet/TestData.xlsx
+++ b/src/main/resources/InputTestData/DataSheet/TestData.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="102">
   <si>
     <t>RunFlag</t>
   </si>
@@ -326,6 +326,21 @@
   </si>
   <si>
     <t>481</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>328</t>
+  </si>
+  <si>
+    <t>560</t>
+  </si>
+  <si>
+    <t>455</t>
+  </si>
+  <si>
+    <t>55</t>
   </si>
 </sst>
 </file>
@@ -860,7 +875,7 @@
         <v>56</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="AC3" t="s" s="0">
         <v>62</v>

</xml_diff>